<commit_message>
Fixed figure 4 - changed regions - search length 11 nt- added deltaSHAPE
</commit_message>
<xml_diff>
--- a/Data/Map files 35S/average_delta_shape.xlsx
+++ b/Data/Map files 35S/average_delta_shape.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\maran\Desktop\diff_BUM_HMM_Project\Github\diff_BUM_HMM\Data\Map files 35S\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85F570FA-D3A6-44D1-83D1-87C76C645912}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C80B42F3-36BE-4B56-870F-F28780106F0E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="21840" windowHeight="13740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -358,15 +358,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Y1647"/>
+  <dimension ref="A1:AP1647"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E105" workbookViewId="0">
-      <selection activeCell="X3" sqref="X3:Y133"/>
+    <sheetView tabSelected="1" topLeftCell="W1" workbookViewId="0">
+      <selection activeCell="AO3" sqref="AO3:AP26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -380,7 +380,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>19</v>
       </c>
@@ -411,8 +411,20 @@
       <c r="W2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AC2">
+        <v>1</v>
+      </c>
+      <c r="AD2">
+        <v>2</v>
+      </c>
+      <c r="AK2">
+        <v>1</v>
+      </c>
+      <c r="AL2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>20</v>
       </c>
@@ -463,8 +475,46 @@
       <c r="Y3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AB3">
+        <v>462</v>
+      </c>
+      <c r="AC3">
+        <v>0</v>
+      </c>
+      <c r="AD3">
+        <v>0</v>
+      </c>
+      <c r="AE3">
+        <f>AVERAGE(AC3:AD3)</f>
+        <v>0</v>
+      </c>
+      <c r="AF3">
+        <v>462</v>
+      </c>
+      <c r="AG3">
+        <v>0</v>
+      </c>
+      <c r="AJ3">
+        <v>2443</v>
+      </c>
+      <c r="AK3">
+        <v>0.103183065465</v>
+      </c>
+      <c r="AL3" s="1">
+        <v>9.7265014238300004E-5</v>
+      </c>
+      <c r="AM3">
+        <f>AVERAGE(AK3:AL3)</f>
+        <v>5.1640165239619153E-2</v>
+      </c>
+      <c r="AO3">
+        <v>2443</v>
+      </c>
+      <c r="AP3">
+        <v>5.1640165239619153E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>21</v>
       </c>
@@ -487,7 +537,7 @@
         <v>0</v>
       </c>
       <c r="O4">
-        <f t="shared" ref="O4:Q67" si="0">AVERAGE(M4:N4)</f>
+        <f t="shared" ref="O4:O67" si="0">AVERAGE(M4:N4)</f>
         <v>0</v>
       </c>
       <c r="P4">
@@ -506,7 +556,7 @@
         <v>0</v>
       </c>
       <c r="W4">
-        <f t="shared" ref="W4:Y67" si="1">AVERAGE(U4:V4)</f>
+        <f t="shared" ref="W4:W67" si="1">AVERAGE(U4:V4)</f>
         <v>0</v>
       </c>
       <c r="X4">
@@ -515,8 +565,46 @@
       <c r="Y4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AB4">
+        <v>463</v>
+      </c>
+      <c r="AC4">
+        <v>7.0157327174299997E-2</v>
+      </c>
+      <c r="AD4">
+        <v>0</v>
+      </c>
+      <c r="AE4">
+        <f>AC4</f>
+        <v>7.0157327174299997E-2</v>
+      </c>
+      <c r="AF4">
+        <v>463</v>
+      </c>
+      <c r="AG4">
+        <v>7.0157327174299997E-2</v>
+      </c>
+      <c r="AJ4">
+        <v>2444</v>
+      </c>
+      <c r="AK4">
+        <v>0.12568771607599999</v>
+      </c>
+      <c r="AL4">
+        <v>1.5914209963699999E-4</v>
+      </c>
+      <c r="AM4">
+        <f t="shared" ref="AM4:AM26" si="2">AVERAGE(AK4:AL4)</f>
+        <v>6.2923429087818492E-2</v>
+      </c>
+      <c r="AO4">
+        <v>2444</v>
+      </c>
+      <c r="AP4">
+        <v>6.2923429087818492E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>22</v>
       </c>
@@ -567,8 +655,46 @@
       <c r="Y5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AB5">
+        <v>464</v>
+      </c>
+      <c r="AC5">
+        <v>0</v>
+      </c>
+      <c r="AD5">
+        <v>0</v>
+      </c>
+      <c r="AE5">
+        <f t="shared" ref="AE4:AE37" si="3">AVERAGE(AC5:AD5)</f>
+        <v>0</v>
+      </c>
+      <c r="AF5">
+        <v>464</v>
+      </c>
+      <c r="AG5">
+        <v>0</v>
+      </c>
+      <c r="AJ5">
+        <v>2445</v>
+      </c>
+      <c r="AK5">
+        <v>9.8630470900800002E-2</v>
+      </c>
+      <c r="AL5">
+        <v>1.71584585423E-4</v>
+      </c>
+      <c r="AM5">
+        <f t="shared" si="2"/>
+        <v>4.9401027743111503E-2</v>
+      </c>
+      <c r="AO5">
+        <v>2445</v>
+      </c>
+      <c r="AP5">
+        <v>4.9401027743111503E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>23</v>
       </c>
@@ -619,8 +745,46 @@
       <c r="Y6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AB6">
+        <v>465</v>
+      </c>
+      <c r="AC6">
+        <v>8.8927585513099996E-2</v>
+      </c>
+      <c r="AD6">
+        <v>0</v>
+      </c>
+      <c r="AE6">
+        <f>AC6</f>
+        <v>8.8927585513099996E-2</v>
+      </c>
+      <c r="AF6">
+        <v>465</v>
+      </c>
+      <c r="AG6">
+        <v>8.8927585513099996E-2</v>
+      </c>
+      <c r="AJ6">
+        <v>2446</v>
+      </c>
+      <c r="AK6">
+        <v>9.5845485425199994E-2</v>
+      </c>
+      <c r="AL6">
+        <v>1.5758084883399999E-4</v>
+      </c>
+      <c r="AM6">
+        <f t="shared" si="2"/>
+        <v>4.8001533137016994E-2</v>
+      </c>
+      <c r="AO6">
+        <v>2446</v>
+      </c>
+      <c r="AP6">
+        <v>4.8001533137016994E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>24</v>
       </c>
@@ -671,8 +835,46 @@
       <c r="Y7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AB7">
+        <v>466</v>
+      </c>
+      <c r="AC7">
+        <v>6.5865082459799995E-2</v>
+      </c>
+      <c r="AD7">
+        <v>0</v>
+      </c>
+      <c r="AE7">
+        <f>AC7</f>
+        <v>6.5865082459799995E-2</v>
+      </c>
+      <c r="AF7">
+        <v>466</v>
+      </c>
+      <c r="AG7">
+        <v>6.5865082459799995E-2</v>
+      </c>
+      <c r="AJ7">
+        <v>2447</v>
+      </c>
+      <c r="AK7">
+        <v>8.6533400611899999E-2</v>
+      </c>
+      <c r="AL7">
+        <v>1.3036486930599999E-4</v>
+      </c>
+      <c r="AM7">
+        <f t="shared" si="2"/>
+        <v>4.3331882740602998E-2</v>
+      </c>
+      <c r="AO7">
+        <v>2447</v>
+      </c>
+      <c r="AP7">
+        <v>4.3331882740602998E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>32</v>
       </c>
@@ -695,7 +897,7 @@
         <v>0</v>
       </c>
       <c r="O8">
-        <f t="shared" ref="O8:Q9" si="2">M8</f>
+        <f t="shared" ref="O8:O9" si="4">M8</f>
         <v>8.1639173275599997E-2</v>
       </c>
       <c r="P8">
@@ -723,8 +925,46 @@
       <c r="Y8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AB8">
+        <v>467</v>
+      </c>
+      <c r="AC8">
+        <v>0</v>
+      </c>
+      <c r="AD8" s="1">
+        <v>-6.7068269933400002E-5</v>
+      </c>
+      <c r="AE8" s="1">
+        <f>AD8</f>
+        <v>-6.7068269933400002E-5</v>
+      </c>
+      <c r="AF8">
+        <v>467</v>
+      </c>
+      <c r="AG8">
+        <v>-6.7068269933400002E-5</v>
+      </c>
+      <c r="AJ8">
+        <v>2448</v>
+      </c>
+      <c r="AK8">
+        <v>9.1431759570400006E-2</v>
+      </c>
+      <c r="AL8">
+        <v>1.1101366708799999E-4</v>
+      </c>
+      <c r="AM8">
+        <f t="shared" si="2"/>
+        <v>4.5771386618744005E-2</v>
+      </c>
+      <c r="AO8">
+        <v>2448</v>
+      </c>
+      <c r="AP8">
+        <v>4.5771386618744005E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>33</v>
       </c>
@@ -747,7 +987,7 @@
         <v>0</v>
       </c>
       <c r="O9">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v>8.6475159990700004E-2</v>
       </c>
       <c r="P9">
@@ -775,8 +1015,46 @@
       <c r="Y9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AB9">
+        <v>468</v>
+      </c>
+      <c r="AC9">
+        <v>0</v>
+      </c>
+      <c r="AD9" s="1">
+        <v>-6.0243467350599998E-5</v>
+      </c>
+      <c r="AE9" s="1">
+        <f>AD9</f>
+        <v>-6.0243467350599998E-5</v>
+      </c>
+      <c r="AF9">
+        <v>468</v>
+      </c>
+      <c r="AG9">
+        <v>-6.0243467350599998E-5</v>
+      </c>
+      <c r="AJ9">
+        <v>2449</v>
+      </c>
+      <c r="AK9">
+        <v>7.4206641009399998E-2</v>
+      </c>
+      <c r="AL9">
+        <v>1.0161395756699999E-4</v>
+      </c>
+      <c r="AM9">
+        <f t="shared" si="2"/>
+        <v>3.7154127483483498E-2</v>
+      </c>
+      <c r="AO9">
+        <v>2449</v>
+      </c>
+      <c r="AP9">
+        <v>3.7154127483483498E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>34</v>
       </c>
@@ -827,8 +1105,46 @@
       <c r="Y10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AB10">
+        <v>469</v>
+      </c>
+      <c r="AC10">
+        <v>0.105424816127</v>
+      </c>
+      <c r="AD10">
+        <v>0</v>
+      </c>
+      <c r="AE10">
+        <f>AC10</f>
+        <v>0.105424816127</v>
+      </c>
+      <c r="AF10">
+        <v>469</v>
+      </c>
+      <c r="AG10">
+        <v>0.105424816127</v>
+      </c>
+      <c r="AJ10">
+        <v>2450</v>
+      </c>
+      <c r="AK10">
+        <v>0</v>
+      </c>
+      <c r="AL10">
+        <v>0</v>
+      </c>
+      <c r="AM10">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AO10">
+        <v>2450</v>
+      </c>
+      <c r="AP10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>35</v>
       </c>
@@ -879,8 +1195,46 @@
       <c r="Y11">
         <v>-6.1543938247900004E-5</v>
       </c>
-    </row>
-    <row r="12" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AB11">
+        <v>470</v>
+      </c>
+      <c r="AC11">
+        <v>0.188351244152</v>
+      </c>
+      <c r="AD11" s="1">
+        <v>9.9578544670900004E-5</v>
+      </c>
+      <c r="AE11">
+        <f t="shared" si="3"/>
+        <v>9.4225411348335453E-2</v>
+      </c>
+      <c r="AF11">
+        <v>470</v>
+      </c>
+      <c r="AG11">
+        <v>9.4225411348335453E-2</v>
+      </c>
+      <c r="AJ11">
+        <v>2451</v>
+      </c>
+      <c r="AK11">
+        <v>0</v>
+      </c>
+      <c r="AL11">
+        <v>0</v>
+      </c>
+      <c r="AM11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AO11">
+        <v>2451</v>
+      </c>
+      <c r="AP11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>36</v>
       </c>
@@ -922,7 +1276,7 @@
         <v>-8.0346305758999994E-5</v>
       </c>
       <c r="W12" s="1">
-        <f t="shared" ref="W12:Y21" si="3">V12</f>
+        <f t="shared" ref="W12:W21" si="5">V12</f>
         <v>-8.0346305758999994E-5</v>
       </c>
       <c r="X12">
@@ -931,8 +1285,46 @@
       <c r="Y12">
         <v>-8.0346305758999994E-5</v>
       </c>
-    </row>
-    <row r="13" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AB12">
+        <v>471</v>
+      </c>
+      <c r="AC12">
+        <v>0.26659256943499998</v>
+      </c>
+      <c r="AD12">
+        <v>1.83263002966E-4</v>
+      </c>
+      <c r="AE12">
+        <f t="shared" si="3"/>
+        <v>0.13338791621898299</v>
+      </c>
+      <c r="AF12">
+        <v>471</v>
+      </c>
+      <c r="AG12">
+        <v>0.13338791621898299</v>
+      </c>
+      <c r="AJ12">
+        <v>2452</v>
+      </c>
+      <c r="AK12">
+        <v>9.3836317484399995E-2</v>
+      </c>
+      <c r="AL12">
+        <v>1.11343357117E-4</v>
+      </c>
+      <c r="AM12">
+        <f t="shared" si="2"/>
+        <v>4.6973830420758499E-2</v>
+      </c>
+      <c r="AO12">
+        <v>2452</v>
+      </c>
+      <c r="AP12">
+        <v>4.6973830420758499E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>37</v>
       </c>
@@ -974,7 +1366,7 @@
         <v>-1.0846411680099999E-4</v>
       </c>
       <c r="W13" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-1.0846411680099999E-4</v>
       </c>
       <c r="X13">
@@ -983,8 +1375,46 @@
       <c r="Y13">
         <v>-1.0846411680099999E-4</v>
       </c>
-    </row>
-    <row r="14" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AB13">
+        <v>472</v>
+      </c>
+      <c r="AC13">
+        <v>0.28899241735800002</v>
+      </c>
+      <c r="AD13">
+        <v>2.11432412249E-4</v>
+      </c>
+      <c r="AE13">
+        <f t="shared" si="3"/>
+        <v>0.14460192488512452</v>
+      </c>
+      <c r="AF13">
+        <v>472</v>
+      </c>
+      <c r="AG13">
+        <v>0.14460192488512452</v>
+      </c>
+      <c r="AJ13">
+        <v>2453</v>
+      </c>
+      <c r="AK13">
+        <v>0.13312253258599999</v>
+      </c>
+      <c r="AL13">
+        <v>2.43463507131E-4</v>
+      </c>
+      <c r="AM13">
+        <f t="shared" si="2"/>
+        <v>6.6682998046565495E-2</v>
+      </c>
+      <c r="AO13">
+        <v>2453</v>
+      </c>
+      <c r="AP13">
+        <v>6.6682998046565495E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>38</v>
       </c>
@@ -1026,7 +1456,7 @@
         <v>-1.5743512726700001E-4</v>
       </c>
       <c r="W14" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-1.5743512726700001E-4</v>
       </c>
       <c r="X14">
@@ -1035,8 +1465,46 @@
       <c r="Y14">
         <v>-1.5743512726700001E-4</v>
       </c>
-    </row>
-    <row r="15" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AB14">
+        <v>473</v>
+      </c>
+      <c r="AC14">
+        <v>0.305333622385</v>
+      </c>
+      <c r="AD14">
+        <v>2.43202023262E-4</v>
+      </c>
+      <c r="AE14">
+        <f t="shared" si="3"/>
+        <v>0.152788412204131</v>
+      </c>
+      <c r="AF14">
+        <v>473</v>
+      </c>
+      <c r="AG14">
+        <v>0.152788412204131</v>
+      </c>
+      <c r="AJ14">
+        <v>2454</v>
+      </c>
+      <c r="AK14">
+        <v>0.174179200384</v>
+      </c>
+      <c r="AL14">
+        <v>3.7273248837500002E-4</v>
+      </c>
+      <c r="AM14">
+        <f t="shared" si="2"/>
+        <v>8.7275966436187499E-2</v>
+      </c>
+      <c r="AO14">
+        <v>2454</v>
+      </c>
+      <c r="AP14">
+        <v>8.7275966436187499E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>39</v>
       </c>
@@ -1078,7 +1546,7 @@
         <v>-1.8803377929000001E-4</v>
       </c>
       <c r="W15" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-1.8803377929000001E-4</v>
       </c>
       <c r="X15">
@@ -1087,8 +1555,46 @@
       <c r="Y15">
         <v>-1.8803377929000001E-4</v>
       </c>
-    </row>
-    <row r="16" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AB15">
+        <v>474</v>
+      </c>
+      <c r="AC15">
+        <v>0.29012277094599997</v>
+      </c>
+      <c r="AD15">
+        <v>2.3464038250600001E-4</v>
+      </c>
+      <c r="AE15">
+        <f t="shared" si="3"/>
+        <v>0.14517870566425298</v>
+      </c>
+      <c r="AF15">
+        <v>474</v>
+      </c>
+      <c r="AG15">
+        <v>0.14517870566425298</v>
+      </c>
+      <c r="AJ15">
+        <v>2455</v>
+      </c>
+      <c r="AK15">
+        <v>0.184094131322</v>
+      </c>
+      <c r="AL15">
+        <v>4.1837203979399999E-4</v>
+      </c>
+      <c r="AM15">
+        <f t="shared" si="2"/>
+        <v>9.2256251680897003E-2</v>
+      </c>
+      <c r="AO15">
+        <v>2455</v>
+      </c>
+      <c r="AP15">
+        <v>9.2256251680897003E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>41</v>
       </c>
@@ -1130,7 +1636,7 @@
         <v>-1.8703635114999999E-4</v>
       </c>
       <c r="W16" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-1.8703635114999999E-4</v>
       </c>
       <c r="X16">
@@ -1139,8 +1645,46 @@
       <c r="Y16">
         <v>-1.8703635114999999E-4</v>
       </c>
-    </row>
-    <row r="17" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AB16">
+        <v>475</v>
+      </c>
+      <c r="AC16">
+        <v>0.27100345276499999</v>
+      </c>
+      <c r="AD16">
+        <v>2.0790317705700001E-4</v>
+      </c>
+      <c r="AE16">
+        <f t="shared" si="3"/>
+        <v>0.13560567797102849</v>
+      </c>
+      <c r="AF16">
+        <v>475</v>
+      </c>
+      <c r="AG16">
+        <v>0.13560567797102849</v>
+      </c>
+      <c r="AJ16">
+        <v>2456</v>
+      </c>
+      <c r="AK16">
+        <v>0.17513054025300001</v>
+      </c>
+      <c r="AL16">
+        <v>3.4653863627300002E-4</v>
+      </c>
+      <c r="AM16">
+        <f t="shared" si="2"/>
+        <v>8.7738539444636512E-2</v>
+      </c>
+      <c r="AO16">
+        <v>2456</v>
+      </c>
+      <c r="AP16">
+        <v>8.7738539444636512E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>42</v>
       </c>
@@ -1182,7 +1726,7 @@
         <v>-1.13720640206E-4</v>
       </c>
       <c r="W17" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-1.13720640206E-4</v>
       </c>
       <c r="X17">
@@ -1191,8 +1735,46 @@
       <c r="Y17">
         <v>-1.13720640206E-4</v>
       </c>
-    </row>
-    <row r="18" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AB17">
+        <v>476</v>
+      </c>
+      <c r="AC17">
+        <v>0.24241834417300001</v>
+      </c>
+      <c r="AD17">
+        <v>1.82665251718E-4</v>
+      </c>
+      <c r="AE17">
+        <f t="shared" si="3"/>
+        <v>0.12130050471235901</v>
+      </c>
+      <c r="AF17">
+        <v>476</v>
+      </c>
+      <c r="AG17">
+        <v>0.12130050471235901</v>
+      </c>
+      <c r="AJ17">
+        <v>2457</v>
+      </c>
+      <c r="AK17">
+        <v>0.16416087529100001</v>
+      </c>
+      <c r="AL17">
+        <v>2.76566359568E-4</v>
+      </c>
+      <c r="AM17">
+        <f t="shared" si="2"/>
+        <v>8.2218720825284003E-2</v>
+      </c>
+      <c r="AO17">
+        <v>2457</v>
+      </c>
+      <c r="AP17">
+        <v>8.2218720825284003E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>43</v>
       </c>
@@ -1215,7 +1797,7 @@
         <v>0</v>
       </c>
       <c r="O18">
-        <f t="shared" ref="O18:Q19" si="4">M18</f>
+        <f t="shared" ref="O18:O19" si="6">M18</f>
         <v>9.3368559439700002E-2</v>
       </c>
       <c r="P18">
@@ -1234,7 +1816,7 @@
         <v>-7.0190664882300004E-5</v>
       </c>
       <c r="W18" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-7.0190664882300004E-5</v>
       </c>
       <c r="X18">
@@ -1243,8 +1825,46 @@
       <c r="Y18">
         <v>-7.0190664882300004E-5</v>
       </c>
-    </row>
-    <row r="19" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AB18">
+        <v>477</v>
+      </c>
+      <c r="AC18">
+        <v>0.22518884104</v>
+      </c>
+      <c r="AD18">
+        <v>1.4752867185900001E-4</v>
+      </c>
+      <c r="AE18">
+        <f t="shared" si="3"/>
+        <v>0.1126681848559295</v>
+      </c>
+      <c r="AF18">
+        <v>477</v>
+      </c>
+      <c r="AG18">
+        <v>0.1126681848559295</v>
+      </c>
+      <c r="AJ18">
+        <v>2458</v>
+      </c>
+      <c r="AK18">
+        <v>0.16168184548600001</v>
+      </c>
+      <c r="AL18">
+        <v>2.4741960392499999E-4</v>
+      </c>
+      <c r="AM18">
+        <f t="shared" si="2"/>
+        <v>8.09646325449625E-2</v>
+      </c>
+      <c r="AO18">
+        <v>2458</v>
+      </c>
+      <c r="AP18">
+        <v>8.09646325449625E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>44</v>
       </c>
@@ -1267,7 +1887,7 @@
         <v>0</v>
       </c>
       <c r="O19">
-        <f t="shared" si="4"/>
+        <f t="shared" si="6"/>
         <v>8.0102420830300003E-2</v>
       </c>
       <c r="P19">
@@ -1286,7 +1906,7 @@
         <v>-6.1242551665999999E-5</v>
       </c>
       <c r="W19" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-6.1242551665999999E-5</v>
       </c>
       <c r="X19">
@@ -1295,8 +1915,46 @@
       <c r="Y19">
         <v>-6.1242551665999999E-5</v>
       </c>
-    </row>
-    <row r="20" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AB19">
+        <v>478</v>
+      </c>
+      <c r="AC19">
+        <v>0.17374802859800001</v>
+      </c>
+      <c r="AD19" s="1">
+        <v>9.3792468802E-5</v>
+      </c>
+      <c r="AE19">
+        <f t="shared" si="3"/>
+        <v>8.6920910533401008E-2</v>
+      </c>
+      <c r="AF19">
+        <v>478</v>
+      </c>
+      <c r="AG19">
+        <v>8.6920910533401008E-2</v>
+      </c>
+      <c r="AJ19">
+        <v>2459</v>
+      </c>
+      <c r="AK19">
+        <v>0.16087650886800001</v>
+      </c>
+      <c r="AL19">
+        <v>2.7642731278400002E-4</v>
+      </c>
+      <c r="AM19">
+        <f t="shared" si="2"/>
+        <v>8.0576468090391998E-2</v>
+      </c>
+      <c r="AO19">
+        <v>2459</v>
+      </c>
+      <c r="AP19">
+        <v>8.0576468090391998E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>45</v>
       </c>
@@ -1338,7 +1996,7 @@
         <v>-7.5152378685999999E-5</v>
       </c>
       <c r="W20" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-7.5152378685999999E-5</v>
       </c>
       <c r="X20">
@@ -1347,8 +2005,46 @@
       <c r="Y20">
         <v>-7.5152378685999999E-5</v>
       </c>
-    </row>
-    <row r="21" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AB20">
+        <v>479</v>
+      </c>
+      <c r="AC20">
+        <v>0.117702389028</v>
+      </c>
+      <c r="AD20">
+        <v>0</v>
+      </c>
+      <c r="AE20">
+        <f>AC20</f>
+        <v>0.117702389028</v>
+      </c>
+      <c r="AF20">
+        <v>479</v>
+      </c>
+      <c r="AG20">
+        <v>0.117702389028</v>
+      </c>
+      <c r="AJ20">
+        <v>2460</v>
+      </c>
+      <c r="AK20">
+        <v>0.15318952603899999</v>
+      </c>
+      <c r="AL20">
+        <v>3.0233874303700002E-4</v>
+      </c>
+      <c r="AM20">
+        <f t="shared" si="2"/>
+        <v>7.6745932391018498E-2</v>
+      </c>
+      <c r="AO20">
+        <v>2460</v>
+      </c>
+      <c r="AP20">
+        <v>7.6745932391018498E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>46</v>
       </c>
@@ -1390,7 +2086,7 @@
         <v>-7.3303540426599995E-5</v>
       </c>
       <c r="W21" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="5"/>
         <v>-7.3303540426599995E-5</v>
       </c>
       <c r="X21">
@@ -1399,8 +2095,46 @@
       <c r="Y21">
         <v>-7.3303540426599995E-5</v>
       </c>
-    </row>
-    <row r="22" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AB21">
+        <v>480</v>
+      </c>
+      <c r="AC21">
+        <v>0</v>
+      </c>
+      <c r="AD21">
+        <v>0</v>
+      </c>
+      <c r="AE21">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AF21">
+        <v>480</v>
+      </c>
+      <c r="AG21">
+        <v>0</v>
+      </c>
+      <c r="AJ21">
+        <v>2461</v>
+      </c>
+      <c r="AK21">
+        <v>0.13053194619</v>
+      </c>
+      <c r="AL21">
+        <v>2.7829844970999999E-4</v>
+      </c>
+      <c r="AM21">
+        <f t="shared" si="2"/>
+        <v>6.5405122319855E-2</v>
+      </c>
+      <c r="AO21">
+        <v>2461</v>
+      </c>
+      <c r="AP21">
+        <v>6.5405122319855E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>47</v>
       </c>
@@ -1451,8 +2185,46 @@
       <c r="Y22">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AB22">
+        <v>481</v>
+      </c>
+      <c r="AC22">
+        <v>0</v>
+      </c>
+      <c r="AD22" s="1">
+        <v>-5.9434152142399997E-5</v>
+      </c>
+      <c r="AE22" s="1">
+        <f>AD22</f>
+        <v>-5.9434152142399997E-5</v>
+      </c>
+      <c r="AF22">
+        <v>481</v>
+      </c>
+      <c r="AG22">
+        <v>-5.9434152142399997E-5</v>
+      </c>
+      <c r="AJ22">
+        <v>2462</v>
+      </c>
+      <c r="AK22">
+        <v>0.11469727767100001</v>
+      </c>
+      <c r="AL22">
+        <v>2.1664244392000001E-4</v>
+      </c>
+      <c r="AM22">
+        <f t="shared" si="2"/>
+        <v>5.7456960057460003E-2</v>
+      </c>
+      <c r="AO22">
+        <v>2462</v>
+      </c>
+      <c r="AP22">
+        <v>5.7456960057460003E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>48</v>
       </c>
@@ -1503,8 +2275,46 @@
       <c r="Y23">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AB23">
+        <v>482</v>
+      </c>
+      <c r="AC23">
+        <v>0</v>
+      </c>
+      <c r="AD23">
+        <v>-1.08776334639E-4</v>
+      </c>
+      <c r="AE23" s="1">
+        <f t="shared" ref="AE23:AE35" si="7">AD23</f>
+        <v>-1.08776334639E-4</v>
+      </c>
+      <c r="AF23">
+        <v>482</v>
+      </c>
+      <c r="AG23">
+        <v>-1.08776334639E-4</v>
+      </c>
+      <c r="AJ23">
+        <v>2463</v>
+      </c>
+      <c r="AK23">
+        <v>8.8290208679500007E-2</v>
+      </c>
+      <c r="AL23">
+        <v>1.27237295994E-4</v>
+      </c>
+      <c r="AM23">
+        <f t="shared" si="2"/>
+        <v>4.4208722987747001E-2</v>
+      </c>
+      <c r="AO23">
+        <v>2463</v>
+      </c>
+      <c r="AP23">
+        <v>4.4208722987747001E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>49</v>
       </c>
@@ -1555,8 +2365,46 @@
       <c r="Y24">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AB24">
+        <v>483</v>
+      </c>
+      <c r="AC24">
+        <v>0</v>
+      </c>
+      <c r="AD24">
+        <v>-1.7204240415700001E-4</v>
+      </c>
+      <c r="AE24" s="1">
+        <f t="shared" si="7"/>
+        <v>-1.7204240415700001E-4</v>
+      </c>
+      <c r="AF24">
+        <v>483</v>
+      </c>
+      <c r="AG24">
+        <v>-1.7204240415700001E-4</v>
+      </c>
+      <c r="AJ24">
+        <v>2464</v>
+      </c>
+      <c r="AK24">
+        <v>6.5964537107099999E-2</v>
+      </c>
+      <c r="AL24">
+        <v>0</v>
+      </c>
+      <c r="AM24">
+        <f>AK24</f>
+        <v>6.5964537107099999E-2</v>
+      </c>
+      <c r="AO24">
+        <v>2464</v>
+      </c>
+      <c r="AP24">
+        <v>6.5964537107099999E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>76</v>
       </c>
@@ -1607,8 +2455,46 @@
       <c r="Y25">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AB25">
+        <v>484</v>
+      </c>
+      <c r="AC25">
+        <v>0</v>
+      </c>
+      <c r="AD25">
+        <v>-1.6901741377900001E-4</v>
+      </c>
+      <c r="AE25" s="1">
+        <f t="shared" si="7"/>
+        <v>-1.6901741377900001E-4</v>
+      </c>
+      <c r="AF25">
+        <v>484</v>
+      </c>
+      <c r="AG25">
+        <v>-1.6901741377900001E-4</v>
+      </c>
+      <c r="AJ25">
+        <v>2465</v>
+      </c>
+      <c r="AK25">
+        <v>0</v>
+      </c>
+      <c r="AL25">
+        <v>0</v>
+      </c>
+      <c r="AM25">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AO25">
+        <v>2465</v>
+      </c>
+      <c r="AP25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>77</v>
       </c>
@@ -1659,8 +2545,46 @@
       <c r="Y26">
         <v>-6.8796458420600007E-5</v>
       </c>
-    </row>
-    <row r="27" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AB26">
+        <v>485</v>
+      </c>
+      <c r="AC26">
+        <v>0</v>
+      </c>
+      <c r="AD26">
+        <v>-1.7044003909600001E-4</v>
+      </c>
+      <c r="AE26" s="1">
+        <f t="shared" si="7"/>
+        <v>-1.7044003909600001E-4</v>
+      </c>
+      <c r="AF26">
+        <v>485</v>
+      </c>
+      <c r="AG26">
+        <v>-1.7044003909600001E-4</v>
+      </c>
+      <c r="AJ26">
+        <v>2466</v>
+      </c>
+      <c r="AK26">
+        <v>0</v>
+      </c>
+      <c r="AL26">
+        <v>0</v>
+      </c>
+      <c r="AM26">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="AO26">
+        <v>2466</v>
+      </c>
+      <c r="AP26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>78</v>
       </c>
@@ -1702,7 +2626,7 @@
         <v>-1.3617042687200001E-4</v>
       </c>
       <c r="W27" s="1">
-        <f t="shared" ref="W27:Y32" si="5">V27</f>
+        <f t="shared" ref="W27:W32" si="8">V27</f>
         <v>-1.3617042687200001E-4</v>
       </c>
       <c r="X27">
@@ -1711,8 +2635,27 @@
       <c r="Y27">
         <v>-1.3617042687200001E-4</v>
       </c>
-    </row>
-    <row r="28" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AB27">
+        <v>486</v>
+      </c>
+      <c r="AC27">
+        <v>0</v>
+      </c>
+      <c r="AD27">
+        <v>-1.5310568084300001E-4</v>
+      </c>
+      <c r="AE27" s="1">
+        <f t="shared" si="7"/>
+        <v>-1.5310568084300001E-4</v>
+      </c>
+      <c r="AF27">
+        <v>486</v>
+      </c>
+      <c r="AG27">
+        <v>-1.5310568084300001E-4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>79</v>
       </c>
@@ -1754,7 +2697,7 @@
         <v>-1.53612895862E-4</v>
       </c>
       <c r="W28" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>-1.53612895862E-4</v>
       </c>
       <c r="X28">
@@ -1763,8 +2706,27 @@
       <c r="Y28">
         <v>-1.53612895862E-4</v>
       </c>
-    </row>
-    <row r="29" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AB28">
+        <v>487</v>
+      </c>
+      <c r="AC28">
+        <v>0</v>
+      </c>
+      <c r="AD28">
+        <v>-2.1609848326599999E-4</v>
+      </c>
+      <c r="AE28" s="1">
+        <f t="shared" si="7"/>
+        <v>-2.1609848326599999E-4</v>
+      </c>
+      <c r="AF28">
+        <v>487</v>
+      </c>
+      <c r="AG28">
+        <v>-2.1609848326599999E-4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>92</v>
       </c>
@@ -1806,7 +2768,7 @@
         <v>-1.59292466411E-4</v>
       </c>
       <c r="W29" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>-1.59292466411E-4</v>
       </c>
       <c r="X29">
@@ -1815,8 +2777,27 @@
       <c r="Y29">
         <v>-1.59292466411E-4</v>
       </c>
-    </row>
-    <row r="30" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AB29">
+        <v>488</v>
+      </c>
+      <c r="AC29">
+        <v>0</v>
+      </c>
+      <c r="AD29">
+        <v>-1.8211559044600001E-4</v>
+      </c>
+      <c r="AE29" s="1">
+        <f t="shared" si="7"/>
+        <v>-1.8211559044600001E-4</v>
+      </c>
+      <c r="AF29">
+        <v>488</v>
+      </c>
+      <c r="AG29">
+        <v>-1.8211559044600001E-4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>93</v>
       </c>
@@ -1858,7 +2839,7 @@
         <v>-1.1023193042599999E-4</v>
       </c>
       <c r="W30" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>-1.1023193042599999E-4</v>
       </c>
       <c r="X30">
@@ -1867,8 +2848,27 @@
       <c r="Y30">
         <v>-1.1023193042599999E-4</v>
       </c>
-    </row>
-    <row r="31" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AB30">
+        <v>489</v>
+      </c>
+      <c r="AC30">
+        <v>0</v>
+      </c>
+      <c r="AD30">
+        <v>-1.4989775337E-4</v>
+      </c>
+      <c r="AE30" s="1">
+        <f t="shared" si="7"/>
+        <v>-1.4989775337E-4</v>
+      </c>
+      <c r="AF30">
+        <v>489</v>
+      </c>
+      <c r="AG30">
+        <v>-1.4989775337E-4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>94</v>
       </c>
@@ -1910,7 +2910,7 @@
         <v>-6.7068269933400002E-5</v>
       </c>
       <c r="W31" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>-6.7068269933400002E-5</v>
       </c>
       <c r="X31">
@@ -1919,8 +2919,27 @@
       <c r="Y31">
         <v>-6.7068269933400002E-5</v>
       </c>
-    </row>
-    <row r="32" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AB31">
+        <v>490</v>
+      </c>
+      <c r="AC31">
+        <v>0</v>
+      </c>
+      <c r="AD31">
+        <v>-1.14640155334E-4</v>
+      </c>
+      <c r="AE31" s="1">
+        <f t="shared" si="7"/>
+        <v>-1.14640155334E-4</v>
+      </c>
+      <c r="AF31">
+        <v>490</v>
+      </c>
+      <c r="AG31">
+        <v>-1.14640155334E-4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:42" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>105</v>
       </c>
@@ -1962,7 +2981,7 @@
         <v>-6.0243467350599998E-5</v>
       </c>
       <c r="W32" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>-6.0243467350599998E-5</v>
       </c>
       <c r="X32">
@@ -1971,8 +2990,27 @@
       <c r="Y32">
         <v>-6.0243467350599998E-5</v>
       </c>
-    </row>
-    <row r="33" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AB32">
+        <v>491</v>
+      </c>
+      <c r="AC32">
+        <v>0</v>
+      </c>
+      <c r="AD32" s="1">
+        <v>-8.40814846462E-5</v>
+      </c>
+      <c r="AE32" s="1">
+        <f t="shared" si="7"/>
+        <v>-8.40814846462E-5</v>
+      </c>
+      <c r="AF32">
+        <v>491</v>
+      </c>
+      <c r="AG32">
+        <v>-8.40814846462E-5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>106</v>
       </c>
@@ -2023,8 +3061,27 @@
       <c r="Y33">
         <v>3.5943247097835446E-2</v>
       </c>
-    </row>
-    <row r="34" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AB33">
+        <v>492</v>
+      </c>
+      <c r="AC33">
+        <v>0</v>
+      </c>
+      <c r="AD33" s="1">
+        <v>-9.2222989908100002E-5</v>
+      </c>
+      <c r="AE33" s="1">
+        <f t="shared" si="7"/>
+        <v>-9.2222989908100002E-5</v>
+      </c>
+      <c r="AF33">
+        <v>492</v>
+      </c>
+      <c r="AG33">
+        <v>-9.2222989908100002E-5</v>
+      </c>
+    </row>
+    <row r="34" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>107</v>
       </c>
@@ -2075,8 +3132,27 @@
       <c r="Y34">
         <v>5.4882359762483006E-2</v>
       </c>
-    </row>
-    <row r="35" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AB34">
+        <v>493</v>
+      </c>
+      <c r="AC34">
+        <v>0</v>
+      </c>
+      <c r="AD34" s="1">
+        <v>-6.0333577528600003E-5</v>
+      </c>
+      <c r="AE34" s="1">
+        <f t="shared" si="7"/>
+        <v>-6.0333577528600003E-5</v>
+      </c>
+      <c r="AF34">
+        <v>493</v>
+      </c>
+      <c r="AG34">
+        <v>-6.0333577528600003E-5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>110</v>
       </c>
@@ -2127,8 +3203,27 @@
       <c r="Y35">
         <v>5.23234004046245E-2</v>
       </c>
-    </row>
-    <row r="36" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AB35">
+        <v>494</v>
+      </c>
+      <c r="AC35">
+        <v>0</v>
+      </c>
+      <c r="AD35" s="1">
+        <v>-6.6744073565699996E-5</v>
+      </c>
+      <c r="AE35" s="1">
+        <f t="shared" si="7"/>
+        <v>-6.6744073565699996E-5</v>
+      </c>
+      <c r="AF35">
+        <v>494</v>
+      </c>
+      <c r="AG35">
+        <v>-6.6744073565699996E-5</v>
+      </c>
+    </row>
+    <row r="36" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>111</v>
       </c>
@@ -2179,8 +3274,27 @@
       <c r="Y36">
         <v>5.5242184307131001E-2</v>
       </c>
-    </row>
-    <row r="37" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AB36">
+        <v>495</v>
+      </c>
+      <c r="AC36">
+        <v>0</v>
+      </c>
+      <c r="AD36" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE36">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AF36">
+        <v>495</v>
+      </c>
+      <c r="AG36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>112</v>
       </c>
@@ -2231,8 +3345,27 @@
       <c r="Y37">
         <v>4.0606444578802997E-2</v>
       </c>
-    </row>
-    <row r="38" spans="1:25" x14ac:dyDescent="0.35">
+      <c r="AB37">
+        <v>496</v>
+      </c>
+      <c r="AC37">
+        <v>0</v>
+      </c>
+      <c r="AD37" s="1">
+        <v>0</v>
+      </c>
+      <c r="AE37">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="AF37">
+        <v>496</v>
+      </c>
+      <c r="AG37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>113</v>
       </c>
@@ -2284,7 +3417,7 @@
         <v>4.2120230185328504E-2</v>
       </c>
     </row>
-    <row r="39" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>114</v>
       </c>
@@ -2336,7 +3469,7 @@
         <v>1.82665251718E-4</v>
       </c>
     </row>
-    <row r="40" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>115</v>
       </c>
@@ -2378,7 +3511,7 @@
         <v>1.4752867185900001E-4</v>
       </c>
       <c r="W40">
-        <f t="shared" ref="W40:Y57" si="6">V40</f>
+        <f t="shared" ref="W40:W57" si="9">V40</f>
         <v>1.4752867185900001E-4</v>
       </c>
       <c r="X40">
@@ -2388,7 +3521,7 @@
         <v>1.4752867185900001E-4</v>
       </c>
     </row>
-    <row r="41" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>116</v>
       </c>
@@ -2430,7 +3563,7 @@
         <v>9.3792468802E-5</v>
       </c>
       <c r="W41">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>9.3792468802E-5</v>
       </c>
       <c r="X41">
@@ -2440,7 +3573,7 @@
         <v>9.3792468802E-5</v>
       </c>
     </row>
-    <row r="42" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>117</v>
       </c>
@@ -2482,7 +3615,7 @@
         <v>-5.9434152142399997E-5</v>
       </c>
       <c r="W42">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>-5.9434152142399997E-5</v>
       </c>
       <c r="X42">
@@ -2492,7 +3625,7 @@
         <v>-5.9434152142399997E-5</v>
       </c>
     </row>
-    <row r="43" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>118</v>
       </c>
@@ -2534,7 +3667,7 @@
         <v>-1.08776334639E-4</v>
       </c>
       <c r="W43">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>-1.08776334639E-4</v>
       </c>
       <c r="X43">
@@ -2544,7 +3677,7 @@
         <v>-1.08776334639E-4</v>
       </c>
     </row>
-    <row r="44" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>119</v>
       </c>
@@ -2586,7 +3719,7 @@
         <v>-1.7204240415700001E-4</v>
       </c>
       <c r="W44">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>-1.7204240415700001E-4</v>
       </c>
       <c r="X44">
@@ -2596,7 +3729,7 @@
         <v>-1.7204240415700001E-4</v>
       </c>
     </row>
-    <row r="45" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A45">
         <v>120</v>
       </c>
@@ -2638,7 +3771,7 @@
         <v>-1.6901741377900001E-4</v>
       </c>
       <c r="W45">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>-1.6901741377900001E-4</v>
       </c>
       <c r="X45">
@@ -2648,7 +3781,7 @@
         <v>-1.6901741377900001E-4</v>
       </c>
     </row>
-    <row r="46" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>125</v>
       </c>
@@ -2690,7 +3823,7 @@
         <v>-1.7044003909600001E-4</v>
       </c>
       <c r="W46">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>-1.7044003909600001E-4</v>
       </c>
       <c r="X46">
@@ -2700,7 +3833,7 @@
         <v>-1.7044003909600001E-4</v>
       </c>
     </row>
-    <row r="47" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>126</v>
       </c>
@@ -2742,7 +3875,7 @@
         <v>-1.5310568084300001E-4</v>
       </c>
       <c r="W47">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>-1.5310568084300001E-4</v>
       </c>
       <c r="X47">
@@ -2752,7 +3885,7 @@
         <v>-1.5310568084300001E-4</v>
       </c>
     </row>
-    <row r="48" spans="1:25" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:33" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>127</v>
       </c>
@@ -2794,7 +3927,7 @@
         <v>-2.1609848326599999E-4</v>
       </c>
       <c r="W48">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>-2.1609848326599999E-4</v>
       </c>
       <c r="X48">
@@ -2846,7 +3979,7 @@
         <v>-1.8211559044600001E-4</v>
       </c>
       <c r="W49">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>-1.8211559044600001E-4</v>
       </c>
       <c r="X49">
@@ -2898,7 +4031,7 @@
         <v>-1.4989775337E-4</v>
       </c>
       <c r="W50">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>-1.4989775337E-4</v>
       </c>
       <c r="X50">
@@ -2950,7 +4083,7 @@
         <v>-1.14640155334E-4</v>
       </c>
       <c r="W51">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>-1.14640155334E-4</v>
       </c>
       <c r="X51">
@@ -3002,7 +4135,7 @@
         <v>-8.40814846462E-5</v>
       </c>
       <c r="W52">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>-8.40814846462E-5</v>
       </c>
       <c r="X52">
@@ -3054,7 +4187,7 @@
         <v>-9.2222989908100002E-5</v>
       </c>
       <c r="W53">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>-9.2222989908100002E-5</v>
       </c>
       <c r="X53">
@@ -3106,7 +4239,7 @@
         <v>-6.0333577528600003E-5</v>
       </c>
       <c r="W54">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>-6.0333577528600003E-5</v>
       </c>
       <c r="X54">
@@ -3158,7 +4291,7 @@
         <v>-6.6744073565699996E-5</v>
       </c>
       <c r="W55">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>-6.6744073565699996E-5</v>
       </c>
       <c r="X55">
@@ -3210,7 +4343,7 @@
         <v>0</v>
       </c>
       <c r="W56">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="X56">
@@ -3262,7 +4395,7 @@
         <v>0</v>
       </c>
       <c r="W57">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
       <c r="X57">
@@ -3607,7 +4740,7 @@
         <v>0</v>
       </c>
       <c r="O64">
-        <f t="shared" ref="O64:Q65" si="7">M64</f>
+        <f t="shared" ref="O64:O65" si="10">M64</f>
         <v>8.6424062701999996E-2</v>
       </c>
       <c r="P64">
@@ -3659,7 +4792,7 @@
         <v>0</v>
       </c>
       <c r="O65">
-        <f t="shared" si="7"/>
+        <f t="shared" si="10"/>
         <v>7.8376778658600002E-2</v>
       </c>
       <c r="P65">
@@ -3815,7 +4948,7 @@
         <v>0</v>
       </c>
       <c r="O68">
-        <f t="shared" ref="O68:Q88" si="8">AVERAGE(M68:N68)</f>
+        <f t="shared" ref="O68:O88" si="11">AVERAGE(M68:N68)</f>
         <v>0</v>
       </c>
       <c r="P68">
@@ -3886,7 +5019,7 @@
         <v>0</v>
       </c>
       <c r="W69">
-        <f t="shared" ref="W69:Y70" si="9">U69</f>
+        <f t="shared" ref="W69:W70" si="12">U69</f>
         <v>6.7797139762200004E-2</v>
       </c>
       <c r="X69">
@@ -3919,7 +5052,7 @@
         <v>0</v>
       </c>
       <c r="O70">
-        <f t="shared" ref="O70:Q71" si="10">M70</f>
+        <f t="shared" ref="O70:O71" si="13">M70</f>
         <v>0.11343992125000001</v>
       </c>
       <c r="P70">
@@ -3938,7 +5071,7 @@
         <v>0</v>
       </c>
       <c r="W70">
-        <f t="shared" si="9"/>
+        <f t="shared" si="12"/>
         <v>8.7494532637099998E-2</v>
       </c>
       <c r="X70">
@@ -3971,7 +5104,7 @@
         <v>0</v>
       </c>
       <c r="O71">
-        <f t="shared" si="10"/>
+        <f t="shared" si="13"/>
         <v>7.65932870579E-2</v>
       </c>
       <c r="P71">
@@ -3990,7 +5123,7 @@
         <v>0</v>
       </c>
       <c r="W71">
-        <f t="shared" ref="W68:Y131" si="11">AVERAGE(U71:V71)</f>
+        <f t="shared" ref="W71:W131" si="14">AVERAGE(U71:V71)</f>
         <v>0</v>
       </c>
       <c r="X71">
@@ -4042,7 +5175,7 @@
         <v>0</v>
       </c>
       <c r="W72">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="X72">
@@ -4094,7 +5227,7 @@
         <v>0</v>
       </c>
       <c r="W73">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="X73">
@@ -4127,7 +5260,7 @@
         <v>-2.5195581937000001E-4</v>
       </c>
       <c r="O74">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>-3.4167868403434998E-2</v>
       </c>
       <c r="P74">
@@ -4146,7 +5279,7 @@
         <v>0</v>
       </c>
       <c r="W74">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="X74">
@@ -4198,7 +5331,7 @@
         <v>0</v>
       </c>
       <c r="W75">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="X75">
@@ -4231,7 +5364,7 @@
         <v>0</v>
       </c>
       <c r="O76">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P76">
@@ -4250,7 +5383,7 @@
         <v>0</v>
       </c>
       <c r="W76">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="X76">
@@ -4283,7 +5416,7 @@
         <v>0</v>
       </c>
       <c r="O77">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P77">
@@ -4302,7 +5435,7 @@
         <v>0</v>
       </c>
       <c r="W77">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="X77">
@@ -4335,7 +5468,7 @@
         <v>0</v>
       </c>
       <c r="O78">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P78">
@@ -4354,7 +5487,7 @@
         <v>0</v>
       </c>
       <c r="W78">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="X78">
@@ -4387,7 +5520,7 @@
         <v>0</v>
       </c>
       <c r="O79">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P79">
@@ -4406,7 +5539,7 @@
         <v>0</v>
       </c>
       <c r="W79">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="X79">
@@ -4439,7 +5572,7 @@
         <v>0</v>
       </c>
       <c r="O80">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P80">
@@ -4491,7 +5624,7 @@
         <v>0</v>
       </c>
       <c r="O81">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P81">
@@ -4510,7 +5643,7 @@
         <v>0</v>
       </c>
       <c r="W81">
-        <f t="shared" ref="W81:Y85" si="12">U81</f>
+        <f t="shared" ref="W81:W85" si="15">U81</f>
         <v>0.11562187319</v>
       </c>
       <c r="X81">
@@ -4562,7 +5695,7 @@
         <v>0</v>
       </c>
       <c r="W82">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0.104459321302</v>
       </c>
       <c r="X82">
@@ -4595,7 +5728,7 @@
         <v>0</v>
       </c>
       <c r="O83">
-        <f t="shared" ref="O83:Q87" si="13">M83</f>
+        <f t="shared" ref="O83:O87" si="16">M83</f>
         <v>9.4513524128900003E-2</v>
       </c>
       <c r="P83">
@@ -4614,7 +5747,7 @@
         <v>0</v>
       </c>
       <c r="W83">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0.104701446076</v>
       </c>
       <c r="X83">
@@ -4647,7 +5780,7 @@
         <v>0</v>
       </c>
       <c r="O84">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>8.3720973979200003E-2</v>
       </c>
       <c r="P84">
@@ -4666,7 +5799,7 @@
         <v>0</v>
       </c>
       <c r="W84">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>0.114348671015</v>
       </c>
       <c r="X84">
@@ -4699,7 +5832,7 @@
         <v>0</v>
       </c>
       <c r="O85">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>0.105418518788</v>
       </c>
       <c r="P85">
@@ -4718,7 +5851,7 @@
         <v>0</v>
       </c>
       <c r="W85">
-        <f t="shared" si="12"/>
+        <f t="shared" si="15"/>
         <v>8.5887887732600005E-2</v>
       </c>
       <c r="X85">
@@ -4751,7 +5884,7 @@
         <v>0</v>
       </c>
       <c r="O86">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>9.1761050081099998E-2</v>
       </c>
       <c r="P86">
@@ -4770,7 +5903,7 @@
         <v>0</v>
       </c>
       <c r="W86">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="X86">
@@ -4803,7 +5936,7 @@
         <v>0</v>
       </c>
       <c r="O87">
-        <f t="shared" si="13"/>
+        <f t="shared" si="16"/>
         <v>7.2718999070299994E-2</v>
       </c>
       <c r="P87">
@@ -4822,7 +5955,7 @@
         <v>0</v>
       </c>
       <c r="W87">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="X87">
@@ -4855,7 +5988,7 @@
         <v>0</v>
       </c>
       <c r="O88">
-        <f t="shared" si="8"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="P88">
@@ -4874,7 +6007,7 @@
         <v>0</v>
       </c>
       <c r="W88">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="X88">
@@ -4908,7 +6041,7 @@
         <v>0</v>
       </c>
       <c r="W89">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="X89">
@@ -4942,7 +6075,7 @@
         <v>0</v>
       </c>
       <c r="W90">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="X90">
@@ -4975,7 +6108,7 @@
         <v>0</v>
       </c>
       <c r="W91">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="X91">
@@ -5008,7 +6141,7 @@
         <v>0</v>
       </c>
       <c r="W92">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="X92">
@@ -5042,7 +6175,7 @@
         <v>0</v>
       </c>
       <c r="W93">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="X93">
@@ -5065,9 +6198,6 @@
       <c r="H94">
         <v>1.1076980998000001E-4</v>
       </c>
-      <c r="I94">
-        <v>281</v>
-      </c>
       <c r="M94" s="1"/>
       <c r="T94">
         <v>461</v>
@@ -5102,9 +6232,6 @@
       <c r="H95">
         <v>1.1520293699000001E-4</v>
       </c>
-      <c r="I95">
-        <v>282</v>
-      </c>
       <c r="T95">
         <v>462</v>
       </c>
@@ -5115,7 +6242,7 @@
         <v>0</v>
       </c>
       <c r="W95">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="X95">
@@ -5138,9 +6265,6 @@
       <c r="H96" s="1">
         <v>9.8821052341700006E-5</v>
       </c>
-      <c r="I96">
-        <v>283</v>
-      </c>
       <c r="M96" s="1"/>
       <c r="T96">
         <v>463</v>
@@ -5169,17 +6293,11 @@
       <c r="C97">
         <v>8.7173256776899993E-2</v>
       </c>
-      <c r="D97">
-        <v>274</v>
-      </c>
       <c r="F97">
         <v>299</v>
       </c>
       <c r="H97">
         <v>1.5879847437900001E-4</v>
-      </c>
-      <c r="I97">
-        <v>299</v>
       </c>
       <c r="M97" s="1"/>
       <c r="T97">
@@ -5192,7 +6310,7 @@
         <v>0</v>
       </c>
       <c r="W97">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="X97">
@@ -5209,17 +6327,11 @@
       <c r="C98">
         <v>8.1639173275599997E-2</v>
       </c>
-      <c r="D98">
-        <v>275</v>
-      </c>
       <c r="F98">
         <v>300</v>
       </c>
       <c r="H98">
         <v>2.09381958028E-4</v>
-      </c>
-      <c r="I98">
-        <v>300</v>
       </c>
       <c r="T98">
         <v>465</v>
@@ -5248,17 +6360,11 @@
       <c r="C99">
         <v>8.6475159990700004E-2</v>
       </c>
-      <c r="D99">
-        <v>276</v>
-      </c>
       <c r="F99">
         <v>301</v>
       </c>
       <c r="H99">
         <v>2.7613144695999998E-4</v>
-      </c>
-      <c r="I99">
-        <v>301</v>
       </c>
       <c r="T99">
         <v>466</v>
@@ -5287,17 +6393,11 @@
       <c r="C100">
         <v>0.14875952674599999</v>
       </c>
-      <c r="D100">
-        <v>281</v>
-      </c>
       <c r="F100">
         <v>302</v>
       </c>
       <c r="H100">
         <v>2.4210463811399999E-4</v>
-      </c>
-      <c r="I100">
-        <v>302</v>
       </c>
       <c r="T100">
         <v>467</v>
@@ -5326,17 +6426,11 @@
       <c r="C101">
         <v>0.17558379069899999</v>
       </c>
-      <c r="D101">
-        <v>282</v>
-      </c>
       <c r="F101">
         <v>303</v>
       </c>
       <c r="H101">
         <v>2.02560274707E-4</v>
-      </c>
-      <c r="I101">
-        <v>303</v>
       </c>
       <c r="T101">
         <v>468</v>
@@ -5365,17 +6459,11 @@
       <c r="C102">
         <v>0.15573188626699999</v>
       </c>
-      <c r="D102">
-        <v>283</v>
-      </c>
       <c r="F102">
         <v>304</v>
       </c>
       <c r="H102">
         <v>1.38562278693E-4</v>
-      </c>
-      <c r="I102">
-        <v>304</v>
       </c>
       <c r="T102">
         <v>469</v>
@@ -5404,17 +6492,11 @@
       <c r="C103">
         <v>0.107110953947</v>
       </c>
-      <c r="D103">
-        <v>284</v>
-      </c>
       <c r="F103">
         <v>314</v>
       </c>
       <c r="H103" s="1">
         <v>7.5865846411599994E-5</v>
-      </c>
-      <c r="I103">
-        <v>314</v>
       </c>
       <c r="M103" s="1"/>
       <c r="T103">
@@ -5444,18 +6526,12 @@
       <c r="C104">
         <v>9.3368559439700002E-2</v>
       </c>
-      <c r="D104">
-        <v>285</v>
-      </c>
       <c r="F104">
         <v>315</v>
       </c>
       <c r="H104" s="1">
         <v>9.9334012465400004E-5</v>
       </c>
-      <c r="I104">
-        <v>315</v>
-      </c>
       <c r="T104">
         <v>471</v>
       </c>
@@ -5466,7 +6542,7 @@
         <v>1.83263002966E-4</v>
       </c>
       <c r="W104">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.13338791621898299</v>
       </c>
       <c r="X104">
@@ -5483,18 +6559,12 @@
       <c r="C105">
         <v>8.0102420830300003E-2</v>
       </c>
-      <c r="D105">
-        <v>286</v>
-      </c>
       <c r="F105">
         <v>316</v>
       </c>
       <c r="H105">
         <v>1.00449929917E-4</v>
       </c>
-      <c r="I105">
-        <v>316</v>
-      </c>
       <c r="T105">
         <v>472</v>
       </c>
@@ -5505,7 +6575,7 @@
         <v>2.11432412249E-4</v>
       </c>
       <c r="W105">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.14460192488512452</v>
       </c>
       <c r="X105">
@@ -5522,17 +6592,11 @@
       <c r="C106">
         <v>6.5170655947E-2</v>
       </c>
-      <c r="D106">
-        <v>297</v>
-      </c>
       <c r="F106">
         <v>317</v>
       </c>
       <c r="H106" s="1">
         <v>9.4081382081400003E-5</v>
-      </c>
-      <c r="I106">
-        <v>317</v>
       </c>
       <c r="M106" s="1"/>
       <c r="T106">
@@ -5545,7 +6609,7 @@
         <v>2.43202023262E-4</v>
       </c>
       <c r="W106">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.152788412204131</v>
       </c>
       <c r="X106">
@@ -5562,18 +6626,12 @@
       <c r="C107">
         <v>9.0158802386899994E-2</v>
       </c>
-      <c r="D107">
-        <v>298</v>
-      </c>
       <c r="F107">
         <v>318</v>
       </c>
       <c r="H107">
         <v>1.02808317583E-4</v>
       </c>
-      <c r="I107">
-        <v>318</v>
-      </c>
       <c r="T107">
         <v>474</v>
       </c>
@@ -5584,7 +6642,7 @@
         <v>2.3464038250600001E-4</v>
       </c>
       <c r="W107">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.14517870566425298</v>
       </c>
       <c r="X107">
@@ -5601,18 +6659,12 @@
       <c r="C108">
         <v>0.15874301233800001</v>
       </c>
-      <c r="D108">
-        <v>299</v>
-      </c>
       <c r="F108">
         <v>319</v>
       </c>
       <c r="H108">
         <v>1.18884851897E-4</v>
       </c>
-      <c r="I108">
-        <v>319</v>
-      </c>
       <c r="T108">
         <v>475</v>
       </c>
@@ -5623,7 +6675,7 @@
         <v>2.0790317705700001E-4</v>
       </c>
       <c r="W108">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.13560567797102849</v>
       </c>
       <c r="X108">
@@ -5640,18 +6692,12 @@
       <c r="C109">
         <v>0.22067696131100001</v>
       </c>
-      <c r="D109">
-        <v>300</v>
-      </c>
       <c r="F109">
         <v>320</v>
       </c>
       <c r="H109">
         <v>1.5069123407800001E-4</v>
       </c>
-      <c r="I109">
-        <v>320</v>
-      </c>
       <c r="T109">
         <v>476</v>
       </c>
@@ -5662,7 +6708,7 @@
         <v>1.82665251718E-4</v>
       </c>
       <c r="W109">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.12130050471235901</v>
       </c>
       <c r="X109">
@@ -5679,18 +6725,12 @@
       <c r="C110">
         <v>0.284178685938</v>
       </c>
-      <c r="D110">
-        <v>301</v>
-      </c>
       <c r="F110">
         <v>321</v>
       </c>
       <c r="H110">
         <v>1.27590053407E-4</v>
       </c>
-      <c r="I110">
-        <v>321</v>
-      </c>
       <c r="T110">
         <v>477</v>
       </c>
@@ -5701,7 +6741,7 @@
         <v>1.4752867185900001E-4</v>
       </c>
       <c r="W110">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0.1126681848559295</v>
       </c>
       <c r="X110">
@@ -5718,17 +6758,11 @@
       <c r="C111">
         <v>0.29310661140900002</v>
       </c>
-      <c r="D111">
-        <v>302</v>
-      </c>
       <c r="F111">
         <v>322</v>
       </c>
       <c r="H111">
         <v>1.08602368484E-4</v>
-      </c>
-      <c r="I111">
-        <v>322</v>
       </c>
       <c r="M111" s="1"/>
       <c r="T111">
@@ -5741,7 +6775,7 @@
         <v>9.3792468802E-5</v>
       </c>
       <c r="W111">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>8.6920910533401008E-2</v>
       </c>
       <c r="X111">
@@ -5758,17 +6792,11 @@
       <c r="C112">
         <v>0.25076054981000001</v>
       </c>
-      <c r="D112">
-        <v>303</v>
-      </c>
       <c r="F112">
         <v>324</v>
       </c>
       <c r="H112" s="1">
         <v>7.7392090997600006E-5</v>
-      </c>
-      <c r="I112">
-        <v>324</v>
       </c>
       <c r="M112" s="1"/>
       <c r="T112">
@@ -5798,17 +6826,11 @@
       <c r="C113">
         <v>0.21149516622600001</v>
       </c>
-      <c r="D113">
-        <v>304</v>
-      </c>
       <c r="F113">
         <v>325</v>
       </c>
       <c r="H113" s="1">
         <v>8.8145601110599993E-5</v>
-      </c>
-      <c r="I113">
-        <v>325</v>
       </c>
       <c r="T113">
         <v>480</v>
@@ -5837,17 +6859,11 @@
       <c r="C114">
         <v>0.114309903911</v>
       </c>
-      <c r="D114">
-        <v>305</v>
-      </c>
       <c r="F114">
         <v>326</v>
       </c>
       <c r="H114">
         <v>1.4589798781699999E-4</v>
-      </c>
-      <c r="I114">
-        <v>326</v>
       </c>
       <c r="M114" s="1"/>
       <c r="T114">
@@ -5877,18 +6893,12 @@
       <c r="C115">
         <v>-7.1578710700700002E-2</v>
       </c>
-      <c r="D115">
-        <v>310</v>
-      </c>
       <c r="F115">
         <v>327</v>
       </c>
       <c r="H115">
         <v>1.69081573607E-4</v>
       </c>
-      <c r="I115">
-        <v>327</v>
-      </c>
       <c r="T115">
         <v>482</v>
       </c>
@@ -5899,7 +6909,7 @@
         <v>-1.08776334639E-4</v>
       </c>
       <c r="W115" s="1">
-        <f t="shared" ref="W115:Y127" si="14">V115</f>
+        <f t="shared" ref="W115:W127" si="17">V115</f>
         <v>-1.08776334639E-4</v>
       </c>
       <c r="X115">
@@ -5916,18 +6926,12 @@
       <c r="C116">
         <v>8.4332065031099995E-2</v>
       </c>
-      <c r="D116">
-        <v>313</v>
-      </c>
       <c r="F116">
         <v>328</v>
       </c>
       <c r="H116">
         <v>1.5383513475600001E-4</v>
       </c>
-      <c r="I116">
-        <v>328</v>
-      </c>
       <c r="T116">
         <v>483</v>
       </c>
@@ -5938,7 +6942,7 @@
         <v>-1.7204240415700001E-4</v>
       </c>
       <c r="W116" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>-1.7204240415700001E-4</v>
       </c>
       <c r="X116">
@@ -5955,17 +6959,11 @@
       <c r="C117">
         <v>0.102294665635</v>
       </c>
-      <c r="D117">
-        <v>314</v>
-      </c>
       <c r="F117">
         <v>329</v>
       </c>
       <c r="H117" s="1">
         <v>7.9786681857399995E-5</v>
-      </c>
-      <c r="I117">
-        <v>329</v>
       </c>
       <c r="M117" s="1"/>
       <c r="T117">
@@ -5978,7 +6976,7 @@
         <v>-1.6901741377900001E-4</v>
       </c>
       <c r="W117" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>-1.6901741377900001E-4</v>
       </c>
       <c r="X117">
@@ -5995,18 +6993,12 @@
       <c r="C118">
         <v>0.113779575548</v>
       </c>
-      <c r="D118">
-        <v>315</v>
-      </c>
       <c r="F118">
         <v>339</v>
       </c>
       <c r="H118">
         <v>-1.6749284653899999E-4</v>
       </c>
-      <c r="I118">
-        <v>339</v>
-      </c>
       <c r="T118">
         <v>485</v>
       </c>
@@ -6017,7 +7009,7 @@
         <v>-1.7044003909600001E-4</v>
       </c>
       <c r="W118" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>-1.7044003909600001E-4</v>
       </c>
       <c r="X118">
@@ -6034,18 +7026,12 @@
       <c r="C119">
         <v>0.111802317323</v>
       </c>
-      <c r="D119">
-        <v>316</v>
-      </c>
       <c r="F119">
         <v>340</v>
       </c>
       <c r="H119">
         <v>-2.7076546252999999E-4</v>
       </c>
-      <c r="I119">
-        <v>340</v>
-      </c>
       <c r="T119">
         <v>486</v>
       </c>
@@ -6056,7 +7042,7 @@
         <v>-1.5310568084300001E-4</v>
       </c>
       <c r="W119" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>-1.5310568084300001E-4</v>
       </c>
       <c r="X119">
@@ -6073,18 +7059,12 @@
       <c r="C120">
         <v>0.102590134571</v>
       </c>
-      <c r="D120">
-        <v>317</v>
-      </c>
       <c r="F120">
         <v>341</v>
       </c>
       <c r="H120">
         <v>-2.5195581937000001E-4</v>
       </c>
-      <c r="I120">
-        <v>341</v>
-      </c>
       <c r="T120">
         <v>487</v>
       </c>
@@ -6095,7 +7075,7 @@
         <v>-2.1609848326599999E-4</v>
       </c>
       <c r="W120" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>-2.1609848326599999E-4</v>
       </c>
       <c r="X120">
@@ -6112,17 +7092,11 @@
       <c r="C121">
         <v>0.12635668055800001</v>
       </c>
-      <c r="D121">
-        <v>318</v>
-      </c>
       <c r="F121">
         <v>342</v>
       </c>
       <c r="H121">
         <v>-1.4303614443899999E-4</v>
-      </c>
-      <c r="I121">
-        <v>342</v>
       </c>
       <c r="M121" s="1"/>
       <c r="T121">
@@ -6135,7 +7109,7 @@
         <v>-1.8211559044600001E-4</v>
       </c>
       <c r="W121" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>-1.8211559044600001E-4</v>
       </c>
       <c r="X121">
@@ -6152,9 +7126,6 @@
       <c r="C122">
         <v>0.127939975648</v>
       </c>
-      <c r="D122">
-        <v>319</v>
-      </c>
       <c r="F122">
         <v>357</v>
       </c>
@@ -6172,7 +7143,7 @@
         <v>-1.4989775337E-4</v>
       </c>
       <c r="W122" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>-1.4989775337E-4</v>
       </c>
       <c r="X122">
@@ -6189,9 +7160,6 @@
       <c r="C123">
         <v>0.142225563961</v>
       </c>
-      <c r="D123">
-        <v>320</v>
-      </c>
       <c r="F123">
         <v>358</v>
       </c>
@@ -6208,7 +7176,7 @@
         <v>-1.14640155334E-4</v>
       </c>
       <c r="W123" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>-1.14640155334E-4</v>
       </c>
       <c r="X123">
@@ -6225,9 +7193,6 @@
       <c r="C124">
         <v>0.10374157356200001</v>
       </c>
-      <c r="D124">
-        <v>321</v>
-      </c>
       <c r="F124">
         <v>359</v>
       </c>
@@ -6245,7 +7210,7 @@
         <v>-8.40814846462E-5</v>
       </c>
       <c r="W124" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>-8.40814846462E-5</v>
       </c>
       <c r="X124">
@@ -6262,17 +7227,11 @@
       <c r="C125">
         <v>7.81819153681E-2</v>
       </c>
-      <c r="D125">
-        <v>322</v>
-      </c>
       <c r="F125">
         <v>378</v>
       </c>
       <c r="H125" s="1">
         <v>-6.1543938247900004E-5</v>
-      </c>
-      <c r="I125">
-        <v>378</v>
       </c>
       <c r="M125" s="1"/>
       <c r="T125">
@@ -6285,7 +7244,7 @@
         <v>-9.2222989908100002E-5</v>
       </c>
       <c r="W125" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>-9.2222989908100002E-5</v>
       </c>
       <c r="X125">
@@ -6302,18 +7261,12 @@
       <c r="C126">
         <v>6.82271178374E-2</v>
       </c>
-      <c r="D126">
-        <v>324</v>
-      </c>
       <c r="F126">
         <v>379</v>
       </c>
       <c r="H126" s="1">
         <v>-8.0346305758999994E-5</v>
       </c>
-      <c r="I126">
-        <v>379</v>
-      </c>
       <c r="T126">
         <v>493</v>
       </c>
@@ -6324,7 +7277,7 @@
         <v>-6.0333577528600003E-5</v>
       </c>
       <c r="W126" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>-6.0333577528600003E-5</v>
       </c>
       <c r="X126">
@@ -6341,17 +7294,11 @@
       <c r="C127">
         <v>9.1928448191100007E-2</v>
       </c>
-      <c r="D127">
-        <v>325</v>
-      </c>
       <c r="F127">
         <v>380</v>
       </c>
       <c r="H127">
         <v>-1.0846411680099999E-4</v>
-      </c>
-      <c r="I127">
-        <v>380</v>
       </c>
       <c r="M127" s="1"/>
       <c r="T127">
@@ -6364,7 +7311,7 @@
         <v>-6.6744073565699996E-5</v>
       </c>
       <c r="W127" s="1">
-        <f t="shared" si="14"/>
+        <f t="shared" si="17"/>
         <v>-6.6744073565699996E-5</v>
       </c>
       <c r="X127">
@@ -6381,18 +7328,12 @@
       <c r="C128">
         <v>0.12926215852799999</v>
       </c>
-      <c r="D128">
-        <v>326</v>
-      </c>
       <c r="F128">
         <v>381</v>
       </c>
       <c r="H128">
         <v>-1.5743512726700001E-4</v>
       </c>
-      <c r="I128">
-        <v>381</v>
-      </c>
       <c r="T128">
         <v>495</v>
       </c>
@@ -6403,7 +7344,7 @@
         <v>0</v>
       </c>
       <c r="W128">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="X128">
@@ -6420,18 +7361,12 @@
       <c r="C129">
         <v>0.16027319681300001</v>
       </c>
-      <c r="D129">
-        <v>327</v>
-      </c>
       <c r="F129">
         <v>382</v>
       </c>
       <c r="H129">
         <v>-1.8803377929000001E-4</v>
       </c>
-      <c r="I129">
-        <v>382</v>
-      </c>
       <c r="T129">
         <v>496</v>
       </c>
@@ -6442,7 +7377,7 @@
         <v>0</v>
       </c>
       <c r="W129">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="X129">
@@ -6459,18 +7394,12 @@
       <c r="C130">
         <v>0.146935968404</v>
       </c>
-      <c r="D130">
-        <v>328</v>
-      </c>
       <c r="F130">
         <v>383</v>
       </c>
       <c r="H130">
         <v>-1.8703635114999999E-4</v>
       </c>
-      <c r="I130">
-        <v>383</v>
-      </c>
       <c r="T130">
         <v>497</v>
       </c>
@@ -6481,7 +7410,7 @@
         <v>0</v>
       </c>
       <c r="W130">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="X130">
@@ -6498,18 +7427,12 @@
       <c r="C131">
         <v>8.9647230711999995E-2</v>
       </c>
-      <c r="D131">
-        <v>329</v>
-      </c>
       <c r="F131">
         <v>384</v>
       </c>
       <c r="H131">
         <v>-1.13720640206E-4</v>
       </c>
-      <c r="I131">
-        <v>384</v>
-      </c>
       <c r="T131">
         <v>498</v>
       </c>
@@ -6520,7 +7443,7 @@
         <v>0</v>
       </c>
       <c r="W131">
-        <f t="shared" si="11"/>
+        <f t="shared" si="14"/>
         <v>0</v>
       </c>
       <c r="X131">
@@ -6537,17 +7460,11 @@
       <c r="C132">
         <v>7.5354587060099995E-2</v>
       </c>
-      <c r="D132">
-        <v>330</v>
-      </c>
       <c r="F132">
         <v>385</v>
       </c>
       <c r="H132" s="1">
         <v>-7.0190664882300004E-5</v>
-      </c>
-      <c r="I132">
-        <v>385</v>
       </c>
       <c r="M132" s="1"/>
       <c r="T132">
@@ -6560,7 +7477,7 @@
         <v>0</v>
       </c>
       <c r="W132">
-        <f t="shared" ref="W132:Y133" si="15">AVERAGE(U132:V132)</f>
+        <f t="shared" ref="W132:W133" si="18">AVERAGE(U132:V132)</f>
         <v>0</v>
       </c>
       <c r="X132">
@@ -6577,17 +7494,11 @@
       <c r="C133">
         <v>8.6424062701999996E-2</v>
       </c>
-      <c r="D133">
-        <v>331</v>
-      </c>
       <c r="F133">
         <v>386</v>
       </c>
       <c r="H133" s="1">
         <v>-6.1242551665999999E-5</v>
-      </c>
-      <c r="I133">
-        <v>386</v>
       </c>
       <c r="M133" s="1"/>
       <c r="T133">
@@ -6600,7 +7511,7 @@
         <v>0</v>
       </c>
       <c r="W133">
-        <f t="shared" si="15"/>
+        <f t="shared" si="18"/>
         <v>0</v>
       </c>
       <c r="X133">
@@ -6617,17 +7528,11 @@
       <c r="C134">
         <v>7.8376778658600002E-2</v>
       </c>
-      <c r="D134">
-        <v>332</v>
-      </c>
       <c r="F134">
         <v>387</v>
       </c>
       <c r="H134" s="1">
         <v>-7.5152378685999999E-5</v>
-      </c>
-      <c r="I134">
-        <v>387</v>
       </c>
     </row>
     <row r="135" spans="1:25" x14ac:dyDescent="0.35">
@@ -6637,17 +7542,11 @@
       <c r="C135">
         <v>8.8564135249999995E-2</v>
       </c>
-      <c r="D135">
-        <v>336</v>
-      </c>
       <c r="F135">
         <v>388</v>
       </c>
       <c r="H135" s="1">
         <v>-7.3303540426599995E-5</v>
-      </c>
-      <c r="I135">
-        <v>388</v>
       </c>
       <c r="M135" s="1"/>
     </row>
@@ -6658,17 +7557,11 @@
       <c r="C136">
         <v>0.11343992125000001</v>
       </c>
-      <c r="D136">
-        <v>337</v>
-      </c>
       <c r="F136">
         <v>393</v>
       </c>
       <c r="H136" s="1">
         <v>-6.8796458420600007E-5</v>
-      </c>
-      <c r="I136">
-        <v>393</v>
       </c>
     </row>
     <row r="137" spans="1:25" x14ac:dyDescent="0.35">
@@ -6678,17 +7571,11 @@
       <c r="C137">
         <v>7.65932870579E-2</v>
       </c>
-      <c r="D137">
-        <v>338</v>
-      </c>
       <c r="F137">
         <v>394</v>
       </c>
       <c r="H137">
         <v>-1.3617042687200001E-4</v>
-      </c>
-      <c r="I137">
-        <v>394</v>
       </c>
     </row>
     <row r="138" spans="1:25" x14ac:dyDescent="0.35">
@@ -6698,17 +7585,11 @@
       <c r="C138">
         <v>-6.8083780987499995E-2</v>
       </c>
-      <c r="D138">
-        <v>341</v>
-      </c>
       <c r="F138">
         <v>395</v>
       </c>
       <c r="H138">
         <v>-1.53612895862E-4</v>
-      </c>
-      <c r="I138">
-        <v>395</v>
       </c>
     </row>
     <row r="139" spans="1:25" x14ac:dyDescent="0.35">
@@ -6718,17 +7599,11 @@
       <c r="C139">
         <v>8.02049899895E-2</v>
       </c>
-      <c r="D139">
-        <v>349</v>
-      </c>
       <c r="F139">
         <v>396</v>
       </c>
       <c r="H139">
         <v>-1.59292466411E-4</v>
-      </c>
-      <c r="I139">
-        <v>396</v>
       </c>
     </row>
     <row r="140" spans="1:25" x14ac:dyDescent="0.35">
@@ -6738,17 +7613,11 @@
       <c r="C140">
         <v>9.4513524128900003E-2</v>
       </c>
-      <c r="D140">
-        <v>350</v>
-      </c>
       <c r="F140">
         <v>397</v>
       </c>
       <c r="H140">
         <v>-1.1023193042599999E-4</v>
-      </c>
-      <c r="I140">
-        <v>397</v>
       </c>
     </row>
     <row r="141" spans="1:25" x14ac:dyDescent="0.35">
@@ -6758,9 +7627,6 @@
       <c r="C141">
         <v>8.3720973979200003E-2</v>
       </c>
-      <c r="D141">
-        <v>351</v>
-      </c>
       <c r="F141">
         <v>467</v>
       </c>
@@ -6779,9 +7645,6 @@
       <c r="C142">
         <v>0.105418518788</v>
       </c>
-      <c r="D142">
-        <v>352</v>
-      </c>
       <c r="F142">
         <v>468</v>
       </c>
@@ -6799,9 +7662,6 @@
       <c r="C143">
         <v>9.1761050081099998E-2</v>
       </c>
-      <c r="D143">
-        <v>353</v>
-      </c>
       <c r="F143">
         <v>470</v>
       </c>
@@ -6819,9 +7679,6 @@
       <c r="C144">
         <v>7.2718999070299994E-2</v>
       </c>
-      <c r="D144">
-        <v>354</v>
-      </c>
       <c r="F144">
         <v>471</v>
       </c>
@@ -6840,9 +7697,6 @@
       <c r="C145">
         <v>7.1786915650999997E-2</v>
       </c>
-      <c r="D145">
-        <v>400</v>
-      </c>
       <c r="F145" s="1">
         <v>472</v>
       </c>
@@ -6860,9 +7714,6 @@
       <c r="C146">
         <v>0.10958145652200001</v>
       </c>
-      <c r="D146">
-        <v>401</v>
-      </c>
       <c r="F146">
         <v>473</v>
       </c>
@@ -6880,9 +7731,6 @@
       <c r="C147">
         <v>0.104435368397</v>
       </c>
-      <c r="D147">
-        <v>402</v>
-      </c>
       <c r="F147">
         <v>474</v>
       </c>
@@ -6900,9 +7748,6 @@
       <c r="C148">
         <v>0.110241166591</v>
       </c>
-      <c r="D148">
-        <v>403</v>
-      </c>
       <c r="F148">
         <v>475</v>
       </c>
@@ -6920,9 +7765,6 @@
       <c r="C149">
         <v>8.0978248775100001E-2</v>
       </c>
-      <c r="D149">
-        <v>404</v>
-      </c>
       <c r="F149">
         <v>476</v>
       </c>
@@ -6940,9 +7782,6 @@
       <c r="C150">
         <v>8.4032557193600005E-2</v>
       </c>
-      <c r="D150">
-        <v>405</v>
-      </c>
       <c r="F150">
         <v>477</v>
       </c>
@@ -6960,9 +7799,6 @@
       <c r="C151">
         <v>6.6904959617400006E-2</v>
       </c>
-      <c r="D151">
-        <v>425</v>
-      </c>
       <c r="F151">
         <v>478</v>
       </c>
@@ -6980,9 +7816,6 @@
       <c r="C152">
         <v>0.10320285742</v>
       </c>
-      <c r="D152">
-        <v>426</v>
-      </c>
       <c r="F152">
         <v>481</v>
       </c>
@@ -7001,9 +7834,6 @@
       <c r="C153">
         <v>9.1481628316799998E-2</v>
       </c>
-      <c r="D153">
-        <v>427</v>
-      </c>
       <c r="F153">
         <v>482</v>
       </c>
@@ -7022,9 +7852,6 @@
       <c r="C154">
         <v>8.4297688533500004E-2</v>
       </c>
-      <c r="D154">
-        <v>428</v>
-      </c>
       <c r="F154">
         <v>483</v>
       </c>
@@ -7042,9 +7869,6 @@
       <c r="C155">
         <v>6.7209681268000004E-2</v>
       </c>
-      <c r="D155">
-        <v>429</v>
-      </c>
       <c r="F155">
         <v>484</v>
       </c>
@@ -7062,9 +7886,6 @@
       <c r="C156">
         <v>7.07218543911E-2</v>
       </c>
-      <c r="D156">
-        <v>435</v>
-      </c>
       <c r="F156">
         <v>485</v>
       </c>
@@ -7083,9 +7904,6 @@
       <c r="C157">
         <v>6.7797139762200004E-2</v>
       </c>
-      <c r="D157">
-        <v>436</v>
-      </c>
       <c r="F157">
         <v>486</v>
       </c>
@@ -7103,9 +7921,6 @@
       <c r="C158">
         <v>8.7494532637099998E-2</v>
       </c>
-      <c r="D158">
-        <v>437</v>
-      </c>
       <c r="F158">
         <v>487</v>
       </c>
@@ -7123,9 +7938,6 @@
       <c r="C159">
         <v>8.0109733957899998E-2</v>
       </c>
-      <c r="D159">
-        <v>447</v>
-      </c>
       <c r="F159">
         <v>488</v>
       </c>
@@ -7143,9 +7955,6 @@
       <c r="C160">
         <v>0.11562187319</v>
       </c>
-      <c r="D160">
-        <v>448</v>
-      </c>
       <c r="F160">
         <v>489</v>
       </c>
@@ -7164,9 +7973,6 @@
       <c r="C161">
         <v>0.104459321302</v>
       </c>
-      <c r="D161">
-        <v>449</v>
-      </c>
       <c r="F161">
         <v>490</v>
       </c>
@@ -7185,9 +7991,6 @@
       <c r="C162">
         <v>0.104701446076</v>
       </c>
-      <c r="D162">
-        <v>450</v>
-      </c>
       <c r="F162">
         <v>491</v>
       </c>
@@ -7205,9 +8008,6 @@
       <c r="C163">
         <v>0.114348671015</v>
       </c>
-      <c r="D163">
-        <v>451</v>
-      </c>
       <c r="F163">
         <v>492</v>
       </c>
@@ -7226,9 +8026,6 @@
       <c r="C164">
         <v>8.5887887732600005E-2</v>
       </c>
-      <c r="D164">
-        <v>452</v>
-      </c>
       <c r="F164">
         <v>493</v>
       </c>
@@ -7246,9 +8043,6 @@
       <c r="C165">
         <v>8.1157732800099996E-2</v>
       </c>
-      <c r="D165">
-        <v>461</v>
-      </c>
       <c r="F165">
         <v>494</v>
       </c>
@@ -8885,6 +9679,9 @@
       <c r="H275" s="1">
         <v>9.7265014238300004E-5</v>
       </c>
+      <c r="I275">
+        <v>2443</v>
+      </c>
     </row>
     <row r="276" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A276">
@@ -8899,6 +9696,9 @@
       <c r="H276">
         <v>1.5914209963699999E-4</v>
       </c>
+      <c r="I276">
+        <v>2444</v>
+      </c>
     </row>
     <row r="277" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A277">
@@ -8913,6 +9713,9 @@
       <c r="H277">
         <v>1.71584585423E-4</v>
       </c>
+      <c r="I277">
+        <v>2445</v>
+      </c>
     </row>
     <row r="278" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A278">
@@ -8927,6 +9730,9 @@
       <c r="H278">
         <v>1.5758084883399999E-4</v>
       </c>
+      <c r="I278">
+        <v>2446</v>
+      </c>
     </row>
     <row r="279" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A279">
@@ -8941,6 +9747,9 @@
       <c r="H279">
         <v>1.3036486930599999E-4</v>
       </c>
+      <c r="I279">
+        <v>2447</v>
+      </c>
       <c r="M279" s="1"/>
     </row>
     <row r="280" spans="1:13" x14ac:dyDescent="0.35">
@@ -8956,6 +9765,9 @@
       <c r="H280">
         <v>1.1101366708799999E-4</v>
       </c>
+      <c r="I280">
+        <v>2448</v>
+      </c>
     </row>
     <row r="281" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A281">
@@ -8970,6 +9782,9 @@
       <c r="H281">
         <v>1.0161395756699999E-4</v>
       </c>
+      <c r="I281">
+        <v>2449</v>
+      </c>
     </row>
     <row r="282" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A282">
@@ -8984,6 +9799,9 @@
       <c r="H282">
         <v>1.11343357117E-4</v>
       </c>
+      <c r="I282">
+        <v>2452</v>
+      </c>
       <c r="M282" s="1"/>
     </row>
     <row r="283" spans="1:13" x14ac:dyDescent="0.35">
@@ -8999,6 +9817,9 @@
       <c r="H283">
         <v>2.43463507131E-4</v>
       </c>
+      <c r="I283">
+        <v>2453</v>
+      </c>
     </row>
     <row r="284" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A284">
@@ -9013,6 +9834,9 @@
       <c r="H284">
         <v>3.7273248837500002E-4</v>
       </c>
+      <c r="I284">
+        <v>2454</v>
+      </c>
     </row>
     <row r="285" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A285">
@@ -9027,6 +9851,9 @@
       <c r="H285">
         <v>4.1837203979399999E-4</v>
       </c>
+      <c r="I285">
+        <v>2455</v>
+      </c>
     </row>
     <row r="286" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A286">
@@ -9041,6 +9868,9 @@
       <c r="H286">
         <v>3.4653863627300002E-4</v>
       </c>
+      <c r="I286">
+        <v>2456</v>
+      </c>
     </row>
     <row r="287" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A287">
@@ -9055,6 +9885,9 @@
       <c r="H287">
         <v>2.76566359568E-4</v>
       </c>
+      <c r="I287">
+        <v>2457</v>
+      </c>
     </row>
     <row r="288" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A288">
@@ -9069,6 +9902,9 @@
       <c r="H288">
         <v>2.4741960392499999E-4</v>
       </c>
+      <c r="I288">
+        <v>2458</v>
+      </c>
     </row>
     <row r="289" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A289">
@@ -9083,6 +9919,9 @@
       <c r="H289">
         <v>2.7642731278400002E-4</v>
       </c>
+      <c r="I289">
+        <v>2459</v>
+      </c>
     </row>
     <row r="290" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A290">
@@ -9097,6 +9936,9 @@
       <c r="H290">
         <v>3.0233874303700002E-4</v>
       </c>
+      <c r="I290">
+        <v>2460</v>
+      </c>
     </row>
     <row r="291" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A291">
@@ -9111,6 +9953,9 @@
       <c r="H291">
         <v>2.7829844970999999E-4</v>
       </c>
+      <c r="I291">
+        <v>2461</v>
+      </c>
     </row>
     <row r="292" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A292">
@@ -9125,6 +9970,9 @@
       <c r="H292">
         <v>2.1664244392000001E-4</v>
       </c>
+      <c r="I292">
+        <v>2462</v>
+      </c>
     </row>
     <row r="293" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A293">
@@ -9139,6 +9987,9 @@
       <c r="H293">
         <v>1.27237295994E-4</v>
       </c>
+      <c r="I293">
+        <v>2463</v>
+      </c>
     </row>
     <row r="294" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A294">
@@ -13420,9 +14271,6 @@
       <c r="A590">
         <v>2443</v>
       </c>
-      <c r="C590">
-        <v>0.103183065465</v>
-      </c>
       <c r="F590">
         <v>5280</v>
       </c>
@@ -13434,9 +14282,6 @@
       <c r="A591">
         <v>2444</v>
       </c>
-      <c r="C591">
-        <v>0.12568771607599999</v>
-      </c>
       <c r="F591">
         <v>5281</v>
       </c>
@@ -13449,9 +14294,6 @@
       <c r="A592">
         <v>2445</v>
       </c>
-      <c r="C592">
-        <v>9.8630470900800002E-2</v>
-      </c>
       <c r="F592">
         <v>5282</v>
       </c>
@@ -13463,9 +14305,6 @@
       <c r="A593">
         <v>2446</v>
       </c>
-      <c r="C593">
-        <v>9.5845485425199994E-2</v>
-      </c>
       <c r="F593">
         <v>5283</v>
       </c>
@@ -13477,9 +14316,6 @@
       <c r="A594">
         <v>2447</v>
       </c>
-      <c r="C594">
-        <v>8.6533400611899999E-2</v>
-      </c>
       <c r="F594">
         <v>5284</v>
       </c>
@@ -13491,9 +14327,6 @@
       <c r="A595">
         <v>2448</v>
       </c>
-      <c r="C595">
-        <v>9.1431759570400006E-2</v>
-      </c>
       <c r="F595">
         <v>5285</v>
       </c>
@@ -13505,9 +14338,6 @@
       <c r="A596">
         <v>2449</v>
       </c>
-      <c r="C596">
-        <v>7.4206641009399998E-2</v>
-      </c>
       <c r="F596">
         <v>5286</v>
       </c>
@@ -13520,9 +14350,6 @@
       <c r="A597">
         <v>2452</v>
       </c>
-      <c r="C597">
-        <v>9.3836317484399995E-2</v>
-      </c>
       <c r="F597">
         <v>5287</v>
       </c>
@@ -13534,9 +14361,6 @@
       <c r="A598">
         <v>2453</v>
       </c>
-      <c r="C598">
-        <v>0.13312253258599999</v>
-      </c>
       <c r="F598">
         <v>5288</v>
       </c>
@@ -13548,9 +14372,6 @@
       <c r="A599">
         <v>2454</v>
       </c>
-      <c r="C599">
-        <v>0.174179200384</v>
-      </c>
       <c r="F599">
         <v>5289</v>
       </c>
@@ -13563,9 +14384,6 @@
       <c r="A600">
         <v>2455</v>
       </c>
-      <c r="C600">
-        <v>0.184094131322</v>
-      </c>
       <c r="F600">
         <v>5341</v>
       </c>
@@ -13578,9 +14396,6 @@
       <c r="A601">
         <v>2456</v>
       </c>
-      <c r="C601">
-        <v>0.17513054025300001</v>
-      </c>
       <c r="F601">
         <v>5342</v>
       </c>
@@ -13592,9 +14407,6 @@
       <c r="A602">
         <v>2457</v>
       </c>
-      <c r="C602">
-        <v>0.16416087529100001</v>
-      </c>
       <c r="F602">
         <v>5343</v>
       </c>
@@ -13606,9 +14418,6 @@
       <c r="A603">
         <v>2458</v>
       </c>
-      <c r="C603">
-        <v>0.16168184548600001</v>
-      </c>
       <c r="F603">
         <v>5361</v>
       </c>
@@ -13621,9 +14430,6 @@
       <c r="A604">
         <v>2459</v>
       </c>
-      <c r="C604">
-        <v>0.16087650886800001</v>
-      </c>
       <c r="F604">
         <v>5362</v>
       </c>
@@ -13635,9 +14441,6 @@
       <c r="A605">
         <v>2460</v>
       </c>
-      <c r="C605">
-        <v>0.15318952603899999</v>
-      </c>
       <c r="F605">
         <v>5363</v>
       </c>
@@ -13649,9 +14452,6 @@
       <c r="A606">
         <v>2461</v>
       </c>
-      <c r="C606">
-        <v>0.13053194619</v>
-      </c>
       <c r="F606">
         <v>5369</v>
       </c>
@@ -13664,9 +14464,6 @@
       <c r="A607">
         <v>2462</v>
       </c>
-      <c r="C607">
-        <v>0.11469727767100001</v>
-      </c>
       <c r="F607">
         <v>5370</v>
       </c>
@@ -13678,9 +14475,6 @@
       <c r="A608">
         <v>2463</v>
       </c>
-      <c r="C608">
-        <v>8.8290208679500007E-2</v>
-      </c>
       <c r="F608">
         <v>5371</v>
       </c>
@@ -13693,9 +14487,6 @@
       <c r="A609">
         <v>2464</v>
       </c>
-      <c r="C609">
-        <v>6.5964537107099999E-2</v>
-      </c>
       <c r="F609">
         <v>5374</v>
       </c>
@@ -22203,6 +22994,18 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="M3:N88">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="U3:V133">
     <cfRule type="colorScale" priority="2">
       <colorScale>
         <cfvo type="min"/>
@@ -22214,7 +23017,7 @@
       </colorScale>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="U3:V133">
+  <conditionalFormatting sqref="AC3:AD37">
     <cfRule type="colorScale" priority="1">
       <colorScale>
         <cfvo type="min"/>

</xml_diff>